<commit_message>
New version of application with more functions
</commit_message>
<xml_diff>
--- a/out/production/QuestInput/sample/CustomerFiles/Excel/EstimateXL.xlsx
+++ b/out/production/QuestInput/sample/CustomerFiles/Excel/EstimateXL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewashley/Documents/IdeaProjects/Quest Input/Customer Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewashley/Documents/IdeaProjects/QuestInput/src/sample/CustomerFiles/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -75,8 +75,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -345,9 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,6 +367,12 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,19 +382,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -411,47 +442,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -761,8 +762,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -775,79 +776,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="31"/>
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="D2" s="9"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="D2" s="44"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6">
@@ -856,215 +857,215 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="15"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="15"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="15"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="15"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="15"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="15"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="15"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="15"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="15"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="15"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="15"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="15"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="15"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="16"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="31" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="12">
+      <c r="F32" s="22"/>
+      <c r="G32" s="11">
         <f>SUM(G9:G31)</f>
         <v>0</v>
       </c>
@@ -1084,6 +1085,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="A32:D32"/>
@@ -1100,26 +1121,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -1131,5 +1132,10 @@
     <oddHeader>&amp;L&amp;"-,Bold"&amp;14 &amp;G          &amp;C&amp;"-,Bold"&amp;14Designquest, LLC&amp;"-,Regular"_x000D_&amp;12 10601 Highway 14_x000D_Gray Court, SC 29645_x000D_864-871-3967_x000D_www.designquest3d.com&amp;R&amp;"-,Bold"&amp;18Estimate</oddHeader>
   </headerFooter>
   <legacyDrawingHF r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>